<commit_message>
Splitting Test suite sheet into module based sheets
adding more test cases to the modules
adding more test data
</commit_message>
<xml_diff>
--- a/Test Requierments Table.xlsx
+++ b/Test Requierments Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB12AB04-48D9-4BA8-8133-2AD6CD5768A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF205A99-5826-4085-8E95-352CC5D5826C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Req. Table" sheetId="7" r:id="rId1"/>
@@ -873,10 +873,12 @@
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -1241,22 +1243,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1268,22 +1270,22 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1602,9 +1604,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8CD782-A754-4D5D-8CA8-D381E0EB2815}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+      <selection pane="topRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="48" customHeight="1"/>
@@ -1673,13 +1675,13 @@
       </c>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="44" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="9" t="s">
         <v>92</v>
       </c>
@@ -1689,29 +1691,29 @@
       <c r="F4" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="33"/>
+      <c r="G4" s="46"/>
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="A5" s="38"/>
+      <c r="A5" s="45"/>
       <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="11" t="s">
         <v>93</v>
       </c>
       <c r="E5" s="41"/>
       <c r="F5" s="40"/>
-      <c r="G5" s="34"/>
+      <c r="G5" s="47"/>
     </row>
     <row r="6" spans="1:7" ht="56.25" customHeight="1">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="42" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="35"/>
+      <c r="C6" s="42"/>
       <c r="D6" s="5" t="s">
         <v>101</v>
       </c>
@@ -1721,20 +1723,20 @@
       <c r="F6" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="G6" s="33"/>
+      <c r="G6" s="46"/>
     </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A7" s="36"/>
+      <c r="A7" s="43"/>
       <c r="B7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="18" t="s">
         <v>102</v>
       </c>
       <c r="E7" s="40"/>
       <c r="F7" s="40"/>
-      <c r="G7" s="34"/>
+      <c r="G7" s="47"/>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
       <c r="A8" s="19" t="s">
@@ -1815,13 +1817,13 @@
       </c>
     </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="60" customHeight="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="44" t="s">
         <v>94</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
@@ -1831,20 +1833,20 @@
       <c r="F13" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="G13" s="33"/>
+      <c r="G13" s="46"/>
     </row>
     <row r="14" spans="1:7" s="14" customFormat="1" ht="60" customHeight="1" thickBot="1">
-      <c r="A14" s="38"/>
+      <c r="A14" s="45"/>
       <c r="B14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="11" t="s">
         <v>96</v>
       </c>
       <c r="E14" s="40"/>
       <c r="F14" s="40"/>
-      <c r="G14" s="34"/>
+      <c r="G14" s="47"/>
     </row>
     <row r="15" spans="1:7" s="22" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
       <c r="A15" s="32" t="s">
@@ -1856,13 +1858,13 @@
       </c>
     </row>
     <row r="16" spans="1:7" s="17" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="44" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="42" t="s">
         <v>120</v>
       </c>
       <c r="D16" s="7" t="s">
@@ -1874,23 +1876,23 @@
       <c r="F16" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="G16" s="33"/>
+      <c r="G16" s="46"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A17" s="38"/>
+      <c r="A17" s="45"/>
       <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="11" t="s">
         <v>99</v>
       </c>
       <c r="E17" s="40"/>
       <c r="F17" s="40"/>
-      <c r="G17" s="34"/>
+      <c r="G17" s="47"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="44" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1908,7 +1910,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="A19" s="38"/>
+      <c r="A19" s="45"/>
       <c r="B19" s="10" t="s">
         <v>91</v>
       </c>
@@ -1945,20 +1947,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G4:G5"/>
@@ -1968,6 +1956,20 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1977,45 +1979,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58265D46-97F3-47F8-8B95-10DCBB576402}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="43"/>
-    <col min="2" max="3" width="14.140625" style="42"/>
-    <col min="4" max="4" width="25.85546875" style="42" customWidth="1"/>
-    <col min="5" max="16384" width="14.140625" style="42"/>
+    <col min="1" max="1" width="14.140625" style="34"/>
+    <col min="2" max="3" width="14.140625" style="33"/>
+    <col min="4" max="4" width="25.85546875" style="33" customWidth="1"/>
+    <col min="5" max="16384" width="14.140625" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="45" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="44" t="s">
+    <row r="1" spans="1:4" s="36" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="47" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="46" t="s">
+    <row r="2" spans="1:4" s="38" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="D2" s="47" t="s">
+      <c r="D2" s="38" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="47" customFormat="1" ht="24" customHeight="1">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:4" s="38" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="37" t="s">
         <v>153</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="38" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Most of the Test Cases are written
login module is the only one left
</commit_message>
<xml_diff>
--- a/Test Requierments Table.xlsx
+++ b/Test Requierments Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF205A99-5826-4085-8E95-352CC5D5826C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46812492-304F-42CF-88B9-002B03F92AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -476,9 +476,6 @@
       </rPr>
       <t>A manager can add a new account for an existing customer.</t>
     </r>
-  </si>
-  <si>
-    <t>Edit Account</t>
   </si>
   <si>
     <r>
@@ -801,6 +798,57 @@
 T81 Email : First character cannot have space</t>
   </si>
   <si>
+    <t>T92 User-ID must not be blank
+T93 Password must not be blank</t>
+  </si>
+  <si>
+    <t>T94 Account No must not be blank
+T95 Special character are not allowed
+T96 Characters are not allowed</t>
+  </si>
+  <si>
+    <t>T97 Old Password must not be blank
+T98 New Password must not be blank
+T99 Enter at-least one numeric value
+T100 Enter at-least one special character
+T101 Choose a difficult Password
+T102 Confirm Password must not be blank
+T103 Passwords do not Match</t>
+  </si>
+  <si>
+    <t>T104 Account No must not be blank
+T105 Special character are not allowed
+T106 Characters are not allowed
+T107 Amount Field must not be blank
+T108 Characters are not allowed
+T109 Special characters are not allowed
+T110 Description cannot be blank</t>
+  </si>
+  <si>
+    <t>Field Type</t>
+  </si>
+  <si>
+    <t>Numerical</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Ristrictions</t>
+  </si>
+  <si>
+    <t>Not Empty</t>
+  </si>
+  <si>
+    <t>No Characters</t>
+  </si>
+  <si>
+    <t>No special characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>T82 Payers Account Number must not be blank
 T83 Special characters are not allowed
 T84 Characters are not allowed
@@ -808,63 +856,16 @@
 T86 Special characters are not allowed
 T87 Characters are not allowed
 T88 Amount Field must not be blank
-T89 Characters are not allowedT90 Special characters are not allowed
+T89 Characters are not allowed
+T90 Special characters are not allowed
 T91 Description cannot be blank</t>
-  </si>
-  <si>
-    <t>T92 User-ID must not be blank
-T93 Password must not be blank</t>
-  </si>
-  <si>
-    <t>T94 Account No must not be blank
-T95 Special character are not allowed
-T96 Characters are not allowed</t>
-  </si>
-  <si>
-    <t>T97 Old Password must not be blank
-T98 New Password must not be blank
-T99 Enter at-least one numeric value
-T100 Enter at-least one special character
-T101 Choose a difficult Password
-T102 Confirm Password must not be blank
-T103 Passwords do not Match</t>
-  </si>
-  <si>
-    <t>T104 Account No must not be blank
-T105 Special character are not allowed
-T106 Characters are not allowed
-T107 Amount Field must not be blank
-T108 Characters are not allowed
-T109 Special characters are not allowed
-T110 Description cannot be blank</t>
-  </si>
-  <si>
-    <t>Field Type</t>
-  </si>
-  <si>
-    <t>Numerical</t>
-  </si>
-  <si>
-    <t>String</t>
-  </si>
-  <si>
-    <t>Ristrictions</t>
-  </si>
-  <si>
-    <t>Not Empty</t>
-  </si>
-  <si>
-    <t>No Characters</t>
-  </si>
-  <si>
-    <t>No special characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -904,8 +905,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -924,6 +932,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="17">
     <border>
@@ -1140,10 +1153,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1213,9 +1227,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1261,6 +1272,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1270,26 +1293,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1604,9 +1628,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8CD782-A754-4D5D-8CA8-D381E0EB2815}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="48" customHeight="1"/>
@@ -1615,31 +1639,31 @@
     <col min="2" max="2" width="12.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="63.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="68.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="26" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" style="26" customWidth="1"/>
     <col min="7" max="16384" width="38.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="25" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7" s="24" customFormat="1" ht="42" customHeight="1" thickBot="1">
+      <c r="A1" s="23" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="26"/>
+      <c r="E1" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="25"/>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="45" t="s">
         <v>107</v>
       </c>
       <c r="B2" s="20" t="s">
@@ -1649,15 +1673,15 @@
       <c r="D2" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="F2" s="29" t="s">
-        <v>136</v>
+      <c r="E2" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="22" customFormat="1" ht="336" customHeight="1" thickBot="1">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="45" t="s">
         <v>106</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -1665,234 +1689,234 @@
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="21" t="s">
-        <v>121</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>137</v>
+        <v>120</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="46" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="40"/>
       <c r="D4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="46"/>
+      <c r="E4" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F4" s="42" t="s">
+        <v>137</v>
+      </c>
+      <c r="G4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="A5" s="45"/>
+      <c r="A5" s="47"/>
       <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="43"/>
+      <c r="C5" s="41"/>
       <c r="D5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="47"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="1:7" ht="56.25" customHeight="1">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="48" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="42"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="39" t="s">
-        <v>126</v>
-      </c>
-      <c r="F6" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="G6" s="46"/>
+      <c r="E6" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="G6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="12" customFormat="1" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A7" s="43"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="41"/>
       <c r="D7" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="47"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="1:7" s="22" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
       <c r="A8" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C8" s="20"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29" t="s">
-        <v>141</v>
+      <c r="E8" s="27"/>
+      <c r="F8" s="28" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="22" customFormat="1" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A9" s="19" t="s">
-        <v>111</v>
+      <c r="A9" s="45" t="s">
+        <v>110</v>
       </c>
       <c r="B9" s="20" t="s">
         <v>90</v>
       </c>
       <c r="C9" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="22" customFormat="1" ht="87" customHeight="1" thickBot="1">
+      <c r="A10" s="45" t="s">
         <v>113</v>
-      </c>
-      <c r="E9" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="F9" s="29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="22" customFormat="1" ht="87" customHeight="1" thickBot="1">
-      <c r="A10" s="19" t="s">
-        <v>114</v>
       </c>
       <c r="B10" s="20" t="s">
         <v>90</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="F10" s="29" t="s">
-        <v>143</v>
+        <v>114</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="22" customFormat="1" ht="150" customHeight="1" thickBot="1">
       <c r="A11" s="19" t="s">
-        <v>109</v>
+        <v>156</v>
       </c>
       <c r="B11" s="20" t="s">
         <v>90</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="17" customFormat="1" ht="360.75" customHeight="1" thickBot="1">
+      <c r="A12" s="50" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F12" s="29" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="17" customFormat="1" ht="360.75" customHeight="1" thickBot="1">
-      <c r="A12" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>145</v>
-      </c>
-    </row>
     <row r="13" spans="1:7" s="13" customFormat="1" ht="60" customHeight="1">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="46" t="s">
         <v>94</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="42"/>
+      <c r="C13" s="40"/>
       <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>146</v>
-      </c>
-      <c r="G13" s="46"/>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="60" customHeight="1" thickBot="1">
-      <c r="A14" s="45"/>
+      <c r="E13" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>157</v>
+      </c>
+      <c r="G13" s="38"/>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" ht="74.25" customHeight="1" thickBot="1">
+      <c r="A14" s="47"/>
       <c r="B14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="43"/>
+      <c r="C14" s="41"/>
       <c r="D14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="47"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="39"/>
     </row>
     <row r="15" spans="1:7" s="22" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A15" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="29" t="s">
-        <v>147</v>
+      <c r="A15" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="E15" s="27"/>
+      <c r="F15" s="28" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="17" customFormat="1" ht="37.5" customHeight="1">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="46" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="42" t="s">
-        <v>120</v>
+      <c r="C16" s="40" t="s">
+        <v>119</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="G16" s="46"/>
+      <c r="E16" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" s="14" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
-      <c r="A17" s="45"/>
+      <c r="A17" s="47"/>
       <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="43"/>
+      <c r="C17" s="41"/>
       <c r="D17" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="47"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="39"/>
     </row>
     <row r="18" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="46" t="s">
         <v>103</v>
       </c>
       <c r="B18" s="8" t="s">
@@ -1902,15 +1926,15 @@
       <c r="D18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="39" t="s">
-        <v>124</v>
-      </c>
-      <c r="F18" s="39" t="s">
-        <v>149</v>
+      <c r="E18" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="F18" s="42" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
-      <c r="A19" s="45"/>
+      <c r="A19" s="47"/>
       <c r="B19" s="10" t="s">
         <v>91</v>
       </c>
@@ -1918,35 +1942,49 @@
       <c r="D19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:7" s="22" customFormat="1" ht="88.5" customHeight="1" thickBot="1">
-      <c r="A20" s="19" t="s">
-        <v>116</v>
+      <c r="A20" s="45" t="s">
+        <v>115</v>
       </c>
       <c r="B20" s="20" t="s">
         <v>90</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>150</v>
+        <v>116</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="48" customHeight="1">
-      <c r="B31" s="31"/>
+      <c r="B31" s="30"/>
     </row>
     <row r="35" spans="3:3" ht="48" customHeight="1">
-      <c r="C35" s="31"/>
+      <c r="C35" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G4:G5"/>
@@ -1956,20 +1994,6 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1985,40 +2009,40 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="24" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="34"/>
-    <col min="2" max="3" width="14.140625" style="33"/>
-    <col min="4" max="4" width="25.85546875" style="33" customWidth="1"/>
-    <col min="5" max="16384" width="14.140625" style="33"/>
+    <col min="1" max="1" width="14.140625" style="33"/>
+    <col min="2" max="3" width="14.140625" style="32"/>
+    <col min="4" max="4" width="25.85546875" style="32" customWidth="1"/>
+    <col min="5" max="16384" width="14.140625" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="36" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:4" s="35" customFormat="1" ht="24" customHeight="1">
+      <c r="A1" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="37" customFormat="1" ht="24" customHeight="1">
+      <c r="A2" s="36" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="37" customFormat="1" ht="24" customHeight="1">
+      <c r="A3" s="36" t="s">
         <v>151</v>
       </c>
-      <c r="B1" s="36" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="38" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="37" t="s">
-        <v>152</v>
-      </c>
-      <c r="B2" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="C2" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2" s="38" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="38" customFormat="1" ht="24" customHeight="1">
-      <c r="A3" s="37" t="s">
+      <c r="B3" s="37" t="s">
         <v>153</v>
-      </c>
-      <c r="B3" s="38" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test execution on V1
</commit_message>
<xml_diff>
--- a/Test Requierments Table.xlsx
+++ b/Test Requierments Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My-Python-Hub\GithubRepos\Guru99-SW-Tesing-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46812492-304F-42CF-88B9-002B03F92AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE4D324-9BBD-4FBC-9671-19D11A41F57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -737,9 +737,6 @@
 T39 Number of Transaction – Special character are not allowed
 T40 Number of Transaction - Number of Transaction must not be blank
 T41 Number of Transaction – Character are not allowed</t>
-  </si>
-  <si>
-    <t>Delete Account Form</t>
   </si>
   <si>
     <t>T42 Account No must not be blank
@@ -846,9 +843,6 @@
     <t>No special characters</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>T82 Payers Account Number must not be blank
 T83 Special characters are not allowed
 T84 Characters are not allowed
@@ -860,12 +854,18 @@
 T90 Special characters are not allowed
 T91 Description cannot be blank</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Edit Account</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete Account </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1157,7 +1157,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1215,9 +1215,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1272,16 +1269,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1293,7 +1284,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1302,13 +1302,10 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1628,294 +1625,294 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE8CD782-A754-4D5D-8CA8-D381E0EB2815}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="48" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="38.42578125" defaultRowHeight="48" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="15" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="15" customWidth="1"/>
     <col min="3" max="3" width="47.5703125" style="15" customWidth="1"/>
     <col min="4" max="4" width="63.7109375" style="15" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="26" customWidth="1"/>
-    <col min="6" max="6" width="68.28515625" style="26" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="68.28515625" style="25" customWidth="1"/>
     <col min="7" max="16384" width="38.42578125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="24" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:7" s="23" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="25"/>
-    </row>
-    <row r="2" spans="1:7" s="22" customFormat="1" ht="63.75" customHeight="1" thickBot="1">
-      <c r="A2" s="45" t="s">
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" s="21" customFormat="1" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="27" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="22" customFormat="1" ht="336" customHeight="1" thickBot="1">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:7" s="21" customFormat="1" ht="354" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="27" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
+    <row r="4" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
         <v>89</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C4" s="40"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="F4" s="42" t="s">
+      <c r="F4" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="G4" s="38"/>
-    </row>
-    <row r="5" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
+      <c r="G4" s="48"/>
+    </row>
+    <row r="5" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="47"/>
       <c r="B5" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C5" s="41"/>
+      <c r="C5" s="45"/>
       <c r="D5" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="43"/>
-      <c r="G5" s="39"/>
-    </row>
-    <row r="6" spans="1:7" ht="56.25" customHeight="1">
-      <c r="A6" s="48" t="s">
+      <c r="E5" s="41"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="49"/>
+    </row>
+    <row r="6" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="42" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="40"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="G6" s="38"/>
-    </row>
-    <row r="7" spans="1:7" s="12" customFormat="1" ht="56.25" customHeight="1" thickBot="1">
-      <c r="A7" s="49"/>
+      <c r="G6" s="48"/>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="43"/>
       <c r="B7" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C7" s="41"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="39"/>
-    </row>
-    <row r="8" spans="1:7" s="22" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
-      <c r="A8" s="19" t="s">
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="49"/>
+    </row>
+    <row r="8" spans="1:7" s="21" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="28" t="s">
+    </row>
+    <row r="9" spans="1:7" s="21" customFormat="1" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F9" s="27" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="22" customFormat="1" ht="54.75" customHeight="1" thickBot="1">
-      <c r="A9" s="45" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="20" t="s">
+    <row r="10" spans="1:7" s="21" customFormat="1" ht="94.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="37" t="s">
+        <v>113</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C9" s="20" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="28" t="s">
-        <v>130</v>
-      </c>
-      <c r="F9" s="28" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="F10" s="27" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="22" customFormat="1" ht="87" customHeight="1" thickBot="1">
-      <c r="A10" s="45" t="s">
-        <v>113</v>
-      </c>
-      <c r="B10" s="20" t="s">
+    <row r="11" spans="1:7" s="21" customFormat="1" ht="154.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E10" s="28" t="s">
-        <v>128</v>
-      </c>
-      <c r="F10" s="28" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" s="27" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="22" customFormat="1" ht="150" customHeight="1" thickBot="1">
-      <c r="A11" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="B11" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="E11" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F11" s="28" t="s">
+    <row r="12" spans="1:7" s="17" customFormat="1" ht="369.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="28" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="17" customFormat="1" ht="360.75" customHeight="1" thickBot="1">
-      <c r="A12" s="50" t="s">
-        <v>131</v>
-      </c>
-      <c r="E12" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="F12" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="13" customFormat="1" ht="60" customHeight="1">
+    <row r="13" spans="1:7" s="13" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="46" t="s">
         <v>94</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C13" s="40"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>157</v>
-      </c>
-      <c r="G13" s="38"/>
-    </row>
-    <row r="14" spans="1:7" s="14" customFormat="1" ht="74.25" customHeight="1" thickBot="1">
+      <c r="F13" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="48"/>
+    </row>
+    <row r="14" spans="1:7" s="14" customFormat="1" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C14" s="41"/>
+      <c r="C14" s="45"/>
       <c r="D14" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="39"/>
-    </row>
-    <row r="15" spans="1:7" s="22" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A15" s="31" t="s">
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="49"/>
+    </row>
+    <row r="15" spans="1:7" s="21" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="E15" s="27"/>
-      <c r="F15" s="28" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="17" customFormat="1" ht="37.5" customHeight="1">
+      <c r="E15" s="26"/>
+      <c r="F15" s="27" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="17" customFormat="1" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="46" t="s">
         <v>97</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="44" t="s">
         <v>119</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>146</v>
-      </c>
-      <c r="G16" s="38"/>
-    </row>
-    <row r="17" spans="1:7" s="14" customFormat="1" ht="37.5" customHeight="1" thickBot="1">
+      <c r="F16" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="48"/>
+    </row>
+    <row r="17" spans="1:7" s="14" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="41"/>
+      <c r="C17" s="45"/>
       <c r="D17" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="43"/>
-      <c r="F17" s="43"/>
-      <c r="G17" s="39"/>
-    </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1">
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="49"/>
+    </row>
+    <row r="18" spans="1:7" s="13" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="46" t="s">
         <v>103</v>
       </c>
@@ -1926,14 +1923,14 @@
       <c r="D18" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="42" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1">
+      <c r="F18" s="39" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="14" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="10" t="s">
         <v>91</v>
@@ -1942,49 +1939,35 @@
       <c r="D19" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-    </row>
-    <row r="20" spans="1:7" s="22" customFormat="1" ht="88.5" customHeight="1" thickBot="1">
-      <c r="A20" s="45" t="s">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+    </row>
+    <row r="20" spans="1:7" s="21" customFormat="1" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="21" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="E20" s="28" t="s">
+      <c r="E20" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="48" customHeight="1">
-      <c r="B31" s="30"/>
-    </row>
-    <row r="35" spans="3:3" ht="48" customHeight="1">
-      <c r="C35" s="30"/>
+      <c r="F20" s="27" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="29"/>
+    </row>
+    <row r="35" spans="3:3" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C35" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A16:A17"/>
     <mergeCell ref="G16:G17"/>
     <mergeCell ref="G13:G14"/>
     <mergeCell ref="G4:G5"/>
@@ -1994,6 +1977,20 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="F13:F14"/>
     <mergeCell ref="F16:F17"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E6:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2007,42 +2004,42 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="24" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="33"/>
-    <col min="2" max="3" width="14.140625" style="32"/>
-    <col min="4" max="4" width="25.85546875" style="32" customWidth="1"/>
-    <col min="5" max="16384" width="14.140625" style="32"/>
+    <col min="1" max="1" width="14.140625" style="32"/>
+    <col min="2" max="3" width="14.140625" style="31"/>
+    <col min="4" max="4" width="25.85546875" style="31" customWidth="1"/>
+    <col min="5" max="16384" width="14.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="35" customFormat="1" ht="24" customHeight="1">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:4" s="34" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="36" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="37" customFormat="1" ht="24" customHeight="1">
-      <c r="A2" s="36" t="s">
+      <c r="C2" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="36" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="B2" s="37" t="s">
-        <v>153</v>
-      </c>
-      <c r="C2" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="37" customFormat="1" ht="24" customHeight="1">
-      <c r="A3" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="B3" s="37" t="s">
-        <v>153</v>
+      <c r="B3" s="36" t="s">
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2059,7 +2056,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
@@ -2068,7 +2065,7 @@
     <col min="7" max="19" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2094,7 +2091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2111,7 +2108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
@@ -2125,7 +2122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
@@ -2139,7 +2136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2156,7 +2153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
@@ -2170,7 +2167,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>28</v>
       </c>
@@ -2184,7 +2181,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2201,7 +2198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2215,7 +2212,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2243,7 +2240,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="22.5703125" customWidth="1"/>
@@ -2252,7 +2249,7 @@
     <col min="7" max="19" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2278,7 +2275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>46</v>
       </c>
@@ -2309,7 +2306,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>50</v>
       </c>
@@ -2337,14 +2334,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="3" width="15.140625" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" customWidth="1"/>
     <col min="5" max="20" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2370,7 +2367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2388,7 +2385,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="2" t="s">
         <v>57</v>
       </c>
@@ -2402,12 +2399,12 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>2</v>
       </c>
@@ -2424,7 +2421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>13</v>
       </c>
@@ -2438,7 +2435,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
@@ -2452,7 +2449,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="12.75" customHeight="1">
+    <row r="8" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -2469,7 +2466,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75" customHeight="1">
+    <row r="9" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2483,7 +2480,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.75" customHeight="1">
+    <row r="10" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>28</v>
       </c>
@@ -2497,7 +2494,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.75" customHeight="1">
+    <row r="11" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>4</v>
       </c>
@@ -2514,7 +2511,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75" customHeight="1">
+    <row r="12" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75" customHeight="1">
+    <row r="13" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="2" t="s">
         <v>39</v>
       </c>
@@ -2542,7 +2539,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75" customHeight="1">
+    <row r="14" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>5</v>
       </c>
@@ -2553,12 +2550,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75" customHeight="1">
+    <row r="15" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.75" customHeight="1">
+    <row r="16" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
         <v>62</v>
       </c>
@@ -2577,14 +2574,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="5" width="15.140625" customWidth="1"/>
     <col min="6" max="6" width="21.5703125" customWidth="1"/>
     <col min="7" max="20" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1">
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2610,7 +2607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.75" customHeight="1">
+    <row r="2" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2627,7 +2624,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.75" customHeight="1">
+    <row r="3" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2644,7 +2641,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.75" customHeight="1">
+    <row r="4" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2" t="s">
         <v>71</v>
       </c>
@@ -2658,7 +2655,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75" customHeight="1">
+    <row r="5" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="2" t="s">
         <v>75</v>
       </c>
@@ -2672,7 +2669,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75" customHeight="1">
+    <row r="6" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>79</v>
       </c>
@@ -2686,7 +2683,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75" customHeight="1">
+    <row r="7" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>3</v>
       </c>

</xml_diff>